<commit_message>
feat: Add VnExpressExcelCrawler class for web scraping and saving articles to Excel
</commit_message>
<xml_diff>
--- a/vnexpress_articles.xlsx
+++ b/vnexpress_articles.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,425 +453,340 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Việt Nam hoan nghênh doanh nghiệp Quảng Đông tăng đầu tư hạ tầng</t>
+          <t>Hàng nghìn biệt thự bỏ hoang nơi đất đấu giá 130 triệu một m2</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/viet-nam-hoan-nghenh-doanh-nghiep-quang-dong-tang-dau-tu-ha-tang-4782863.html</t>
+          <t>https://vnexpress.net/hang-nghin-biet-thu-bo-hoang-noi-dat-dau-gia-130-trieu-mot-m2-4784776.html</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Tổng Bí thư, Chủ tịch nước Tô Lâm hoan nghênh doanh nghiệp Quảng Đông mở rộng quy mô đầu tư chất lượng cao vào Việt Nam, như chuyển đổi số, tăng trưởng xanh, cơ sở hạ tầng.</t>
+          <t>Hà NộiThửa đất nền "chưa có gì" ở Hoài Đức được tranh mua xuyên đêm, giá hơn 130 triệu đồng trong khi nhà liền kề, biệt thự xây sẵn gần đó không người ở.</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Thưởng tiền cho học sinh giỏi</t>
+          <t>Trước khi tôi mất tiền…</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/thuong-tien-cho-hoc-sinh-gioi-4782258.html</t>
+          <t>https://vnexpress.net/truoc-khi-toi-mat-tien-4785171.html</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Phần thưởng học sinh giỏi của con tôi, năm nào cũng vậy, thường là phong bì và mấy quyển vở.</t>
+          <t>Đang lướt Facebook, mắt tôi vấp phải đường link bài viết có tiêu đề gây sốc: 'Ngân hàng Nhà nước kiện ông A'.</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Hàng trăm người chờ giật tiền cúng cô hồn</t>
+          <t>Đề xuất xây dựng một đoạn cao tốc Hà Nội - Viêng Chăn</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://video.vnexpress.net/hang-tram-nguoi-cho-giat-tien-cung-co-hon-4782898.html</t>
+          <t>https://vnexpress.net/de-xuat-xay-dung-mot-doan-cao-toc-ha-noi-vieng-chan-4785334.html</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>TP HCMHàng trăm người đứng chờ ở đường Phùng Hưng gần ba giờ để giật tiền, đồ cúng cô hồn, tuy nhiên một số gia đình chỉ phát đồ để hạn chế tranh giành.</t>
+          <t>Dự án cao tốc Hà Nội - Viêng Chăn, đoạn Vinh - Thanh Thủy (Nghệ An) dài 65 km được đề xuất xây dựng với tổng vốn 18.500 tỷ đồng.</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Điểm chuẩn Đại học Y Hà Nội cao nhất 28,83</t>
+          <t>Thông điệp từ chuyến thăm Ukraine của Thủ tướng Ấn Độ</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/diem-chuan-dai-hoc-y-ha-noi-nam-2024-4782124.html</t>
+          <t>https://vnexpress.net/thong-diep-tu-chuyen-tham-ukraine-cua-thu-tuong-an-do-4785116.html</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Đại học Y Hà Nội công bố điểm chuẩn từ 19 đến 28,83, cao nhất là ngành Tâm lý học ở khối C00 (Văn, Sử, Địa).</t>
+          <t>Lần đầu thăm Ukraine, Thủ tướng Modi dường như muốn trấn an phương Tây rằng Ấn Độ không hoàn toàn ngả về Nga như họ vẫn nghĩ.</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Thủ môn Patrick Lê Giang nhận gần 23 tỷ ở CLB TP HCM</t>
+          <t>Cổ vật Hoàng thành Thăng Long trưng bày ở TP HCM</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/thu-mon-patrick-le-giang-nhan-gan-23-ty-o-clb-tp-hcm-4782908.html</t>
+          <t>https://vnexpress.net/co-vat-hoang-thanh-thang-long-trung-bay-o-tp-hcm-4784829.html</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Thủ môn Việt kiều Patrick Lê Giang ký hợp đồng mới với CLB TP CHM trong ba năm, lĩnh lương tháng 450 triệu.</t>
+          <t>150 hiện vật, tài liệu, hình ảnh tại Khu di sản Hoàng thành Thăng Long trưng bày ở Bảo tàng TP HCM, quận 1.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Tài xế bị phạt 11 triệu đồng vì dừng xe đón khách trên cao tốc</t>
+          <t>Arsenal đòi được món nợ từ Aston Villa</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/tai-xe-bi-phat-11-trieu-dong-vi-dung-xe-don-khach-tren-cao-toc-4782901.html</t>
+          <t>https://vnexpress.net/arsenal-doi-duoc-mon-no-tu-aston-villa-4785356.html</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Tài xế 53 tuổi ở TP Lào Cai bị phạt 11 triệu đồng, tước giấy phép lái xe 3 tháng do dừng xe trên cao tốc Hà Nội - Lào Cai để đón khách.</t>
+          <t>AnhTận dụng cơ hội tốt hơn kèm một chút may mắn, thầy trò Mikel Arteta đánh bại đối thủ khó chơi 2-0 ở vòng 2 Ngoại hạng Anh.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Tây Nguyên được đầu tư gần 1.900 km cao tốc</t>
+          <t>Bộ Giáo dục: Thầy cô được đàng hoàng dạy thêm</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/tay-nguyen-duoc-dau-tu-gan-1-900-km-cao-toc-4782867.html</t>
+          <t>https://vnexpress.net/bo-giao-duc-thay-co-duoc-dang-hoang-day-them-4785315.html</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Đăk LăkMục tiêu đến năm 2030, Tây Nguyên sẽ hoàn thành 9 tuyến cao tốc dài gần 1.900 km, thúc đẩy phát triển kinh tế, xã hội của vùng.</t>
+          <t>Thầy cô được đàng hoàng dạy học sinh của mình ngoài nhà trường nhưng tuyệt đối không được ép buộc, theo Vụ trưởng Trung học.</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Miền Bắc mưa giông 4 ngày tới</t>
+          <t>IS nhận trách nhiệm vụ đâm dao tại lễ hội ở Đức</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/mien-bac-mua-giong-4-ngay-toi-4782805.html</t>
+          <t>https://vnexpress.net/is-nhan-trach-nhiem-vu-dam-dao-tai-le-hoi-o-duc-4785362.html</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Sau ít ngày nắng nóng, miền Bắc sẽ mưa giông diện rộng từ đêm nay đến hết ngày 22/8, chủ yếu về đêm và sáng.</t>
+          <t>IS tuyên bố kẻ thực hiện vụ đâm dao khiến ba người chết tại lễ hội ở thành phố Solingen, phía tây Đức, là thành viên của nhóm này.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>An ninh Mỹ lập 'vành đai thép' bảo vệ đại hội đảng Dân chủ</t>
+          <t>iPhone 16 có thể bán tại Việt Nam cuối tháng 9</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/an-ninh-my-lap-vanh-dai-thep-bao-ve-dai-hoi-dang-dan-chu-4782860.html</t>
+          <t>https://vnexpress.net/iphone-16-co-the-ban-tai-viet-nam-cuoi-thang-9-4784978.html</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Cảnh sát Chicago lên kế hoạch siết chặt an ninh, ứng phó mọi mối đe dọa trong 4 ngày đại hội toàn quốc đảng Dân chủ diễn ra ở thành phố.</t>
+          <t>Việt Nam vẫn nằm trong những thị trường ưu tiên thứ hai của Apple và nhiều khả năng sẽ bán iPhone 16 ngay trong tháng 9.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Doanh số các cửa hàng thực phẩm chay tăng gấp đôi mùa Vu Lan</t>
+          <t>Hà Nội phân luồng giao thông dịp nghỉ lễ 2/9</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/doanh-so-cac-cua-hang-thuc-pham-chay-tang-gap-doi-mua-vu-lan-4782792.html</t>
+          <t>https://vnexpress.net/ha-noi-phan-luong-giao-thong-dip-nghi-le-2-9-4785331.html</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Thực phẩm chay mùa Vu Lan đang được ưa chuộng, giúp nhiều cửa hàng tăng doanh số gấp đôi so với các tháng trước.</t>
+          <t>Nhằm hạn chế ùn tắc tại các tuyến đường ra, vào thành phố dịp lễ 2/9, Sở Giao thông Vận tải Hà Nội vừa thông báo hướng dẫn phân luồng.</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>'Bảng giá đất mới sẽ không làm tăng giá nhà ở xã hội'</t>
+          <t>Tiến sĩ hóa học 'bước ra' từ gian bếp nghèo của mẹ</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/bang-gia-dat-moi-se-khong-lam-tang-gia-nha-o-xa-hoi-4782848.html</t>
+          <t>https://vnexpress.net/tien-si-hoa-hoc-buoc-ra-tu-gian-bep-ngheo-cua-me-4784851.html</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>TP HCMBảng giá đất điều chỉnh không làm tăng giá nhà ở xã hội do được miễn tiền sử dụng đất, chi phí cấu thành giá nhà theo cơ chế thị trường, theo Sở Xây dựng TP HCM.</t>
+          <t>Hà NộiNăm 2012, khi nhận bằng tiến sĩ loại xuất sắc, các phóng viên Tây Ban Nha hỏi lý do đến đây học, cô gái Việt Nam Vũ Thị Tần liền bắt đầu câu chuyện từ gian bếp của mẹ.</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Tài tử Alain Delon qua đời</t>
+          <t>Haaland lập hat-trick giúp Man City thắng ngược</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/tai-tu-alain-delon-qua-doi-4782857.html</t>
+          <t>https://vnexpress.net/haaland-lap-hat-trick-giup-man-city-thang-nguoc-4785344.html</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>PhápNgôi sao người Pháp Alain Delon - nổi tiếng với phim "Purple Noon" và "Le Samouraï" - qua đời ở tuổi 89.</t>
+          <t>AnhTiền đạo Erling Haaland lập hat-trick, giúp chủ nhà Man City đè bẹp tân binh Ipswich Town 4-1 ở vòng hai Ngoại hạng Anh.</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Cảnh sát cưỡi ngựa xuyên vòng lửa ở trung tâm TP HCM</t>
+          <t>Chuyến ăn mừng trên du thuyền hóa thảm kịch của tỷ phú Anh</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/canh-sat-cuoi-ngua-xuyen-vong-lua-o-trung-tam-tp-hcm-4782835.html</t>
+          <t>https://vnexpress.net/chuyen-an-mung-tren-du-thuyen-hoa-tham-kich-cua-ty-phu-anh-4785120.html</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>100 chiến sĩ cảnh sát cùng ngựa biểu diễn vượt tường lửa, bắn súng, cướp cờ và võ thuật trên đường Lê Lợi, quận 1, thu hút người dân, du khách, sáng 18/8.</t>
+          <t>Tỷ phú Mike Lynch muốn đi du thuyền khắp Địa Trung Hải để ăn mừng phán quyết vô tội tại Mỹ, nhưng hành trình nhanh chóng biến thành thảm kịch.</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Tâm trạng của lính Nga bị Ukraine bắt làm tù binh ở Kursk</t>
+          <t>Tường San đoạt á hậu Chuyển giới Quốc tế</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/tam-trang-cua-linh-nga-bi-ukraine-bat-lam-tu-binh-o-kursk-4782454.html</t>
+          <t>https://vnexpress.net/tuong-san-doat-a-hau-chuyen-gioi-quoc-te-4785306.html</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Nhiều lính nghĩa vụ Nga từng không nghĩ mình sẽ phải tham chiến và đã rất sợ hãi khi bị Ukraine bắt làm tù binh trong chiến dịch tấn công tỉnh Kursk.</t>
+          <t>Thái LanTường San, 19 tuổi, đoạt danh hiệu á hậu 2 ở chung kết Hoa hậu Chuyển giới Quốc tế lần 18, tối 24/8.</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Điểm chuẩn Đại học Y Dược TP HCM tăng, cao nhất 27,8</t>
+          <t>Thanh niên chết não hiến tạng ghép cho 6 người</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/diem-chuan-dai-hoc-y-duoc-tp-hcm-tang-cao-nhat-27-8-4782840.html</t>
+          <t>https://vnexpress.net/thanh-nien-chet-nao-hien-tang-ghep-cho-6-nguoi-4785312.html</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Điểm chuẩn Đại học Y Dược TP HCM (UMP) tăng ở hầu hết ngành, cao nhất là Y khoa với 27,8 điểm.</t>
+          <t>Hà NộiNam thanh niên 32 tuổi chết não do tai nạn giao thông, hiến hai quả thận, giác mạc, tim, gan, là trường hợp lấy - ghép mô tạng đầu tiên do Bệnh viện Đa khoa Xanh Pôn thực hiện.</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Ôtô lao xuống vực bốc cháy, một người chết</t>
+          <t>Son Heung-min ghi cú đúp khi Tottenham thắng đậm</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/oto-lao-xuong-vuc-boc-chay-mot-nguoi-chet-4782854.html</t>
+          <t>https://vnexpress.net/son-heung-min-ghi-cu-dup-khi-tottenham-thang-dam-4785351.html</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Hà GiangLao xuống vực sâu hơn 50 m ở huyện Yên Minh, xe 5 chỗ bốc cháy khiến một người chết, một người bỏng nặng, rạng sáng 18/8.</t>
+          <t>AnhTiền đạo Hàn Quốc Son Heung-min lập cú đúp, giúp Tottenham thắng đội khách Everton 4-0 ở vòng hai Ngoại hạng Anh.</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Vua Thái Lan phê chuẩn con gái ông Thaksin làm Thủ tướng</t>
+          <t>Cá nhân, chủ hộ kinh doanh nợ thuế có thể bị cấm xuất cảnh</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/vua-thai-lan-phe-chuan-con-gai-ong-thaksin-lam-thu-tuong-4782807.html</t>
+          <t>https://vnexpress.net/ca-nhan-chu-ho-kinh-doanh-no-thue-co-the-bi-cam-xuat-canh-4785309.html</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Quốc vương Thái Lan chính thức bổ nhiệm bà Paetongtarn Shinawatra, 37 tuổi, làm Thủ tướng mới của đất nước.</t>
+          <t>Bộ Tài chính muốn thêm cá nhân, chủ hộ kinh doanh vào đối tượng bị tạm hoãn xuất cảnh do chưa hoàn thành nghĩa vụ thuế.</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Hải Phòng sẽ đập bỏ 16 chung cư cũ làm khu tái định cư</t>
+          <t>Iran muốn kiểm soát tình trạng thù địch với Mỹ</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/hai-phong-se-dap-bo-16-chung-cu-cu-lam-khu-tai-dinh-cu-4782720.html</t>
+          <t>https://vnexpress.net/iran-muon-kiem-soat-tinh-trang-thu-dich-voi-my-4785338.html</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>16 chung cư cũ ở quận Ngô Quyền sẽ được đập bỏ để tạo quỹ đất rộng khoảng 10 ha phục vụ tái định cư, đấu giá và quỹ đất dự phòng.</t>
+          <t>Ngoại trưởng Iran Abbas Araghchi tuyên bố nước này muốn kiểm soát tình trạng thù địch với Mỹ để giảm bớt sức ép và đối phó lệnh trừng phạt.</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>5 trải nghiệm miền Tây cho người trẻ dịp 2/9</t>
+          <t>Chuyên gia: Vị thế của TP HCM đang bị 'xói mòn'</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/5-trai-nghiem-mien-tay-cho-nguoi-tre-dip-2-9-4781921.html</t>
+          <t>https://vnexpress.net/chuyen-gia-vi-the-cua-tp-hcm-dang-bi-xoi-mon-4785273.html</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Cào nghêu ở Tiền Giang, lội bộ qua ba đảo ở Kiên Giang hay check in cánh đồng điện gió Bạc Liêu là những trải nghiệm thiên nhiên cho du khách dịp 2/9.</t>
+          <t>Vị thế của TP HCM đang bị "xói mòn" và đứng trước nhiều thách thức khi so với các địa phương khác và một số đô thị lớn ở Đông Nam Á, theo TS Vũ Thành Tự Anh.</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Ông Trump: Tôi ưa nhìn hơn bà Harris</t>
+          <t>Man Utd thua phút 95 ở Ngoại hạng Anh</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/ong-trump-toi-ua-nhin-hon-ba-harris-4782802.html</t>
+          <t>https://vnexpress.net/man-utd-thua-phut-95-o-ngoai-hang-anh-4785327.html</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Cựu tổng thống Trump nói ông có ngoại hình đẹp hơn Phó tổng thống Harris, tiếp tục công kích cá nhân đối thủ đảng Dân chủ.</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Quốc Trung: 'Nghệ sĩ trẻ gần như không có khát vọng vươn ra quốc tế'</t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>https://vnexpress.net/quoc-trung-nghe-si-tre-gan-nhu-khong-co-khat-vong-vuon-ra-quoc-te-4782544.html</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>Nhạc sĩ Quốc Trung nói tầm nhìn của nghệ sĩ trẻ Việt hiện chỉ gói gọn ở việc bán hàng TikTok, sự nổi tiếng, cơm áo gạo tiền.</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Nhóm điều dưỡng ứng cứu nạn nhân bị lật xe trên cao tốc</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>https://vnexpress.net/nhom-dieu-duong-ung-cuu-nan-nhan-bi-lat-xe-tren-cao-toc-4782826.html</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>Trên đường đi tham quan, nhóm nhân viên y tế thuộc Trung tâm Điều dưỡng người có công Quảng Ninh thấy chiếc xe 16 chỗ bị tai nạn, liền dừng lại cấp cứu.</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>CEO Thế Giới Di Động: Giá đã rẻ, giờ sẽ tìm cách bán được nhiều hơn</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>https://vnexpress.net/ceo-the-gioi-di-dong-gia-da-re-gio-se-tim-cach-ban-duoc-nhieu-hon-4782766.html</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Sếp Thế Giới Di Động nói mặt bằng giá cả đã hợp lý, giờ là lúc công ty dồn ngân sách kích cầu để bán được nhiều điện thoại, điện máy hơn.</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Israel không kích Gaza, 18 người trong một gia đình thiệt mạng</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>https://vnexpress.net/israel-khong-kich-gaza-18-nguoi-trong-mot-gia-dinh-thiet-mang-4782742.html</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Quân đội Israel không kích thị trấn Zawaida ở Gaza, khiến 18 thành viên trong một gia đình thiệt mạng.</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Điểm chuẩn Đại học Sư phạm Hà Nội cao nhất 29,3</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>https://vnexpress.net/diem-chuan-dai-hoc-su-pham-ha-noi-cao-nhat-29-3-4782161.html</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Ngành Sư phạm Ngữ văn và Lịch sử của trường Đại học Sư phạm Hà Nội có điểm chuẩn 29,3, cao nhất trong số các trường đã công bố.</t>
+          <t>AnhMan Utd thất bại 1-2 trước chủ nhà Brighton với bàn thua ở phút bù hiệp hai, trận sớm nhất vòng hai Ngoại hạng Anh.</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chore: Update ChatBotVNExpress.py to allow user-defined maximum number of articles to crawl
</commit_message>
<xml_diff>
--- a/vnexpress_articles.xlsx
+++ b/vnexpress_articles.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,272 +521,102 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Cổ vật Hoàng thành Thăng Long trưng bày ở TP HCM</t>
+          <t>Bộ Giáo dục: Thầy cô được đàng hoàng dạy thêm</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/co-vat-hoang-thanh-thang-long-trung-bay-o-tp-hcm-4784829.html</t>
+          <t>https://vnexpress.net/bo-giao-duc-thay-co-duoc-dang-hoang-day-them-4785315.html</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>150 hiện vật, tài liệu, hình ảnh tại Khu di sản Hoàng thành Thăng Long trưng bày ở Bảo tàng TP HCM, quận 1.</t>
+          <t>Thầy cô được đàng hoàng dạy học sinh của mình ngoài nhà trường nhưng tuyệt đối không được ép buộc, theo Vụ trưởng Trung học.</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Arsenal đòi được món nợ từ Aston Villa</t>
+          <t>Hành trình của CEO Telegram trước khi bị bắt</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/arsenal-doi-duoc-mon-no-tu-aston-villa-4785356.html</t>
+          <t>https://vnexpress.net/hanh-trinh-cua-ceo-telegram-truoc-khi-bi-bat-4785389.html</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>AnhTận dụng cơ hội tốt hơn kèm một chút may mắn, thầy trò Mikel Arteta đánh bại đối thủ khó chơi 2-0 ở vòng 2 Ngoại hạng Anh.</t>
+          <t>Hơn 11 năm sau khi sáng lập Telegram, tỷ phú Pavel Durov bị bắt khi gần chạm giấc mơ một tỷ người dùng hoạt động hàng tháng trên nền tảng.</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Bộ Giáo dục: Thầy cô được đàng hoàng dạy thêm</t>
+          <t>Cổ vật Hoàng thành Thăng Long trưng bày ở TP HCM</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/bo-giao-duc-thay-co-duoc-dang-hoang-day-them-4785315.html</t>
+          <t>https://vnexpress.net/co-vat-hoang-thanh-thang-long-trung-bay-o-tp-hcm-4784829.html</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Thầy cô được đàng hoàng dạy học sinh của mình ngoài nhà trường nhưng tuyệt đối không được ép buộc, theo Vụ trưởng Trung học.</t>
+          <t>150 hiện vật, tài liệu, hình ảnh tại Khu di sản Hoàng thành Thăng Long trưng bày ở Bảo tàng TP HCM, quận 1.</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>IS nhận trách nhiệm vụ đâm dao tại lễ hội ở Đức</t>
+          <t>Arsenal đòi được món nợ từ Aston Villa</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/is-nhan-trach-nhiem-vu-dam-dao-tai-le-hoi-o-duc-4785362.html</t>
+          <t>https://vnexpress.net/arsenal-doi-duoc-mon-no-tu-aston-villa-4785356.html</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>IS tuyên bố kẻ thực hiện vụ đâm dao khiến ba người chết tại lễ hội ở thành phố Solingen, phía tây Đức, là thành viên của nhóm này.</t>
+          <t>AnhTận dụng cơ hội tốt hơn kèm một chút may mắn, thầy trò Mikel Arteta đánh bại đối thủ khó chơi 2-0 ở vòng 2 Ngoại hạng Anh.</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>iPhone 16 có thể bán tại Việt Nam cuối tháng 9</t>
+          <t>IS nhận trách nhiệm vụ đâm dao tại lễ hội ở Đức</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/iphone-16-co-the-ban-tai-viet-nam-cuoi-thang-9-4784978.html</t>
+          <t>https://vnexpress.net/is-nhan-trach-nhiem-vu-dam-dao-tai-le-hoi-o-duc-4785362.html</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Việt Nam vẫn nằm trong những thị trường ưu tiên thứ hai của Apple và nhiều khả năng sẽ bán iPhone 16 ngay trong tháng 9.</t>
+          <t>IS tuyên bố kẻ thực hiện vụ đâm dao khiến ba người chết tại lễ hội ở thành phố Solingen, phía tây Đức, là thành viên của nhóm này.</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Hà Nội phân luồng giao thông dịp nghỉ lễ 2/9</t>
+          <t>iPhone 16 có thể bán tại Việt Nam cuối tháng 9</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://vnexpress.net/ha-noi-phan-luong-giao-thong-dip-nghi-le-2-9-4785331.html</t>
+          <t>https://vnexpress.net/iphone-16-co-the-ban-tai-viet-nam-cuoi-thang-9-4784978.html</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Nhằm hạn chế ùn tắc tại các tuyến đường ra, vào thành phố dịp lễ 2/9, Sở Giao thông Vận tải Hà Nội vừa thông báo hướng dẫn phân luồng.</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Tiến sĩ hóa học 'bước ra' từ gian bếp nghèo của mẹ</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>https://vnexpress.net/tien-si-hoa-hoc-buoc-ra-tu-gian-bep-ngheo-cua-me-4784851.html</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Hà NộiNăm 2012, khi nhận bằng tiến sĩ loại xuất sắc, các phóng viên Tây Ban Nha hỏi lý do đến đây học, cô gái Việt Nam Vũ Thị Tần liền bắt đầu câu chuyện từ gian bếp của mẹ.</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Haaland lập hat-trick giúp Man City thắng ngược</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>https://vnexpress.net/haaland-lap-hat-trick-giup-man-city-thang-nguoc-4785344.html</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>AnhTiền đạo Erling Haaland lập hat-trick, giúp chủ nhà Man City đè bẹp tân binh Ipswich Town 4-1 ở vòng hai Ngoại hạng Anh.</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Chuyến ăn mừng trên du thuyền hóa thảm kịch của tỷ phú Anh</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>https://vnexpress.net/chuyen-an-mung-tren-du-thuyen-hoa-tham-kich-cua-ty-phu-anh-4785120.html</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Tỷ phú Mike Lynch muốn đi du thuyền khắp Địa Trung Hải để ăn mừng phán quyết vô tội tại Mỹ, nhưng hành trình nhanh chóng biến thành thảm kịch.</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Tường San đoạt á hậu Chuyển giới Quốc tế</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>https://vnexpress.net/tuong-san-doat-a-hau-chuyen-gioi-quoc-te-4785306.html</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Thái LanTường San, 19 tuổi, đoạt danh hiệu á hậu 2 ở chung kết Hoa hậu Chuyển giới Quốc tế lần 18, tối 24/8.</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>Thanh niên chết não hiến tạng ghép cho 6 người</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>https://vnexpress.net/thanh-nien-chet-nao-hien-tang-ghep-cho-6-nguoi-4785312.html</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Hà NộiNam thanh niên 32 tuổi chết não do tai nạn giao thông, hiến hai quả thận, giác mạc, tim, gan, là trường hợp lấy - ghép mô tạng đầu tiên do Bệnh viện Đa khoa Xanh Pôn thực hiện.</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Son Heung-min ghi cú đúp khi Tottenham thắng đậm</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>https://vnexpress.net/son-heung-min-ghi-cu-dup-khi-tottenham-thang-dam-4785351.html</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>AnhTiền đạo Hàn Quốc Son Heung-min lập cú đúp, giúp Tottenham thắng đội khách Everton 4-0 ở vòng hai Ngoại hạng Anh.</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Cá nhân, chủ hộ kinh doanh nợ thuế có thể bị cấm xuất cảnh</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>https://vnexpress.net/ca-nhan-chu-ho-kinh-doanh-no-thue-co-the-bi-cam-xuat-canh-4785309.html</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Bộ Tài chính muốn thêm cá nhân, chủ hộ kinh doanh vào đối tượng bị tạm hoãn xuất cảnh do chưa hoàn thành nghĩa vụ thuế.</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>Iran muốn kiểm soát tình trạng thù địch với Mỹ</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>https://vnexpress.net/iran-muon-kiem-soat-tinh-trang-thu-dich-voi-my-4785338.html</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Ngoại trưởng Iran Abbas Araghchi tuyên bố nước này muốn kiểm soát tình trạng thù địch với Mỹ để giảm bớt sức ép và đối phó lệnh trừng phạt.</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>Chuyên gia: Vị thế của TP HCM đang bị 'xói mòn'</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>https://vnexpress.net/chuyen-gia-vi-the-cua-tp-hcm-dang-bi-xoi-mon-4785273.html</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Vị thế của TP HCM đang bị "xói mòn" và đứng trước nhiều thách thức khi so với các địa phương khác và một số đô thị lớn ở Đông Nam Á, theo TS Vũ Thành Tự Anh.</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Man Utd thua phút 95 ở Ngoại hạng Anh</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>https://vnexpress.net/man-utd-thua-phut-95-o-ngoai-hang-anh-4785327.html</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>AnhMan Utd thất bại 1-2 trước chủ nhà Brighton với bàn thua ở phút bù hiệp hai, trận sớm nhất vòng hai Ngoại hạng Anh.</t>
+          <t>Việt Nam vẫn nằm trong những thị trường ưu tiên thứ hai của Apple và nhiều khả năng sẽ bán iPhone 16 ngay trong tháng 9.</t>
         </is>
       </c>
     </row>

</xml_diff>